<commit_message>
modify variables and armor data
</commit_message>
<xml_diff>
--- a/script/armor.xlsx
+++ b/script/armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiayuguo/mhw_pc_armor_editor/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8047FD-256A-B34F-A209-676794F064A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0E99AC-F9DA-9345-9A30-DED3EBC5B92F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="2740" windowWidth="25840" windowHeight="14440" xr2:uid="{AF8F22B8-E06C-064E-B168-BC8F456CDDE4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>target</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,10 +81,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>昂扬护石</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>000000000000000000000000000000350003000000000000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -102,6 +98,202 @@
   </si>
   <si>
     <t>04FDFEFE0301040000AE0001270001310002290001130003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>耳塞护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000000000000000000000000000000B0004000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000000000000000004E00051300040B0004390003140004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>达人护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000000000000000130004000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000000000000000003F00034E0005130004140004040003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000000000000000300004000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000000000000000001300034E00053000041400043E0003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000B100044E00051E0005270002140003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000B100044E00051F0005270002140003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000000000000000000000000000001E0005000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000000000000000000000000000001F0005000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000000000000000200005000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000B100044E0005200005270002140003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000000000000000210005000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000B100044E0005210005270002140003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000000000000000220005000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000B100044E0005220005270002140003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>睡眠护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>麻痹护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>毒护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利刃护石</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>昂扬护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挑战护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁壁护石5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>友爱护石5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>匠护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000000000000000230004000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000AF00043A00032300041300054E0005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000000000000000240004000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000000000000000250004000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000AF00043A00032400041300054E0005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000AF00043A00032500041300054E0005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000000000000000A20001000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000000000000000009C0001650003AB00032F0002380003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000000000000000500005000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000000000000000004E0005130003500005360003B90003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000000000000000520005000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000C700035A0003520005610003780003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000000000000000000000000000003E0004000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000000000000000004E00051300043E0004610003140004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000000000000000000000000000360004000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000000000000000004E00051300033600041400033F0003</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -159,10 +351,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -479,23 +671,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FD5401-EBD4-F440-90F9-87E04DA63BEA}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="50" customWidth="1"/>
+    <col min="1" max="2" width="50" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -503,10 +695,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
@@ -514,10 +706,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
@@ -525,10 +717,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
@@ -536,25 +728,201 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>